<commit_message>
remove turbo links move to rails 5
</commit_message>
<xml_diff>
--- a/laradminModel.xlsx
+++ b/laradminModel.xlsx
@@ -208,8 +208,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -233,7 +235,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -241,6 +243,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -248,6 +251,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -580,7 +584,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -607,7 +611,7 @@
       <c r="D1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>30</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -719,9 +723,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" ht="30">
       <c r="B6" t="s">
         <v>6</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="E6" t="s">
         <v>27</v>
@@ -735,12 +742,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="30">
+    <row r="8" spans="1:12">
       <c r="B8" t="s">
         <v>8</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:12">

</xml_diff>